<commit_message>
Update code for advance sumary + refund export
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/PhieuDeNghiThanhToanTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/PhieuDeNghiThanhToanTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\workspace\ael\src\main\resources\ExportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <r>
       <t>CÔNG TY TNHH THƯƠNG MẠI – DỊCH VỤ</t>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t xml:space="preserve">${employee.address.address} </t>
+  </si>
+  <si>
+    <t>${refundDetails.cont}</t>
   </si>
 </sst>
 </file>
@@ -770,7 +773,7 @@
   <dimension ref="A2:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -871,7 +874,9 @@
       <c r="B14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="10"/>
+      <c r="C14" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="D14" s="10" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
- Update chi phi nhathau - THanh toan
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/PhieuDeNghiThanhToanTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/PhieuDeNghiThanhToanTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\workspace\ael\src\main\resources\ExportTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -50,9 +50,6 @@
     <t xml:space="preserve">Mã số </t>
   </si>
   <si>
-    <t>PHIẾU ĐỀ NGHỊ TẠM ỨNG</t>
-  </si>
-  <si>
     <r>
       <t>Kính g</t>
     </r>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>${refundDetails.cont}</t>
+  </si>
+  <si>
+    <t>PHIẾU ĐỀ NGHỊ THANH TOÁN</t>
   </si>
 </sst>
 </file>
@@ -773,7 +773,7 @@
   <dimension ref="A2:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -809,82 +809,82 @@
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="18">
       <c r="C7" s="6" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75">
       <c r="A8" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75">
       <c r="A9" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75">
       <c r="A10" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="12" t="s">
+      <c r="E13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="F14" s="16" t="s">
         <v>24</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -892,37 +892,37 @@
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="16" t="s">
         <v>26</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75">
       <c r="C16" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="15.75">
       <c r="B17" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="15.75">
       <c r="B18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix template for export phieu de nghi tam ung/ thanh toan
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/PhieuDeNghiThanhToanTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/PhieuDeNghiThanhToanTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20370" windowHeight="7980"/>
+    <workbookView windowWidth="20370" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,12 +176,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -228,11 +228,6 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -313,19 +308,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -352,12 +347,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,11 +670,11 @@
         </a:custGeom>
         <a:gradFill rotWithShape="0">
           <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
+            </a:gs>
             <a:gs pos="100000">
               <a:srgbClr val="9CBEE0"/>
-            </a:gs>
-            <a:gs pos="0">
-              <a:srgbClr val="BBD5F0"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
@@ -705,18 +700,18 @@
   <sheetPr/>
   <dimension ref="A2:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.14285714285714" style="1"/>
-    <col min="2" max="2" width="23.4285714285714" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.4285714285714" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.4285714285714" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.11428571428571" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6380952380952" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.8571428571429" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.2" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.2190476190476" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6095238095238" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.14285714285714" style="1"/>
   </cols>
   <sheetData>
@@ -748,7 +743,7 @@
       <c r="F6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="3"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="3:3">
       <c r="C7" s="7" t="s">
@@ -793,13 +788,13 @@
       <c r="B14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>18</v>
       </c>
       <c r="F14" s="9" t="s">
@@ -807,77 +802,78 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="3:5">
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="3:5">
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="D18" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E18" s="13"/>
     </row>
     <row r="19" spans="2:2">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="14" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>